<commit_message>
files with surveyor names
</commit_message>
<xml_diff>
--- a/data/survival/Westcott/B_survival_06202024.xlsx
+++ b/data/survival/Westcott/B_survival_06202024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/survival/Westcott/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F59268-66CB-C643-BFAB-C55E32B92B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58765C9B-1A32-9244-8541-5341623CF9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="1280" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
+    <workbookView xWindow="8080" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>bag_num</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>dead</t>
+  </si>
+  <si>
+    <t>surveyor</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Erik</t>
   </si>
 </sst>
 </file>
@@ -438,18 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCF0E53-B26D-5F4D-A696-5BB849B2395F}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,10 +469,13 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,8 +485,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -484,8 +499,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -496,10 +514,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -510,10 +531,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -523,8 +547,11 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -534,8 +561,11 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -545,8 +575,11 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -557,10 +590,13 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -571,10 +607,13 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -585,6 +624,9 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>